<commit_message>
python module and packages
</commit_message>
<xml_diff>
--- a/Python Session/python_session.xlsx
+++ b/Python Session/python_session.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="352">
   <si>
     <t>python keyword</t>
   </si>
@@ -1188,6 +1188,9 @@
   </si>
   <si>
     <t>khan102030</t>
+  </si>
+  <si>
+    <t>python -m venv venv310</t>
   </si>
 </sst>
 </file>
@@ -1285,12 +1288,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1299,7 +1317,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1320,6 +1338,7 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1604,8 +1623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1796,8 +1815,8 @@
       <c r="C25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:5" ht="19.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1808,8 +1827,8 @@
       </c>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:5" ht="19.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="16" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1820,7 +1839,7 @@
       </c>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="19.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>23</v>
       </c>
@@ -3541,7 +3560,7 @@
   <dimension ref="A3:B5"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3579,7 +3598,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3658,6 +3677,11 @@
         <v>348</v>
       </c>
     </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>351</v>
+      </c>
+    </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>349</v>

</xml_diff>